<commit_message>
Solicitud atendida: LE_06_08_CO (1 a la 12).
Solicitó editor Cristian
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/LE_06_08_Solicitud_Grafica.xlsx
+++ b/fuentes/contenidos/grado06/guion08/LE_06_08_Solicitud_Grafica.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,12 @@
     <definedName name="Formato">'Solicitud gráfica'!$L$2:$L$3</definedName>
     <definedName name="Ubicación">'Solicitud gráfica'!$M$2:$M$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -669,16 +669,9 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -721,18 +714,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -839,18 +820,13 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -897,6 +873,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="37">
     <border>
@@ -1101,11 +1082,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1114,7 +1095,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1122,17 +1103,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1142,7 +1123,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1150,12 +1131,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1164,18 +1145,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1205,11 +1186,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1219,10 +1200,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color auto="1"/>
@@ -1232,7 +1213,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -1306,16 +1287,16 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1323,23 +1304,23 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1361,112 +1342,112 @@
   </borders>
   <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1484,7 +1465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1505,196 +1486,184 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1724,24 +1693,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="51"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="51" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="51" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="22" fillId="9" borderId="5" xfId="51" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="51"/>
+    <xf numFmtId="1" fontId="22" fillId="9" borderId="5" xfId="51" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="51" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="51" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="51" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="51" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="36" xfId="51" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
+    <cellStyle name="Correcto" xfId="51" builtinId="26"/>
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1767,7 +1751,6 @@
     <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="51" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -1875,7 +1858,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>1092900</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>35240</xdr:rowOff>
+      <xdr:rowOff>56406</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1919,7 +1902,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>2010266</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>100301</xdr:rowOff>
+      <xdr:rowOff>121467</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1962,15 +1945,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1038225</xdr:colOff>
+          <xdr:colOff>1041400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1983,7 +1966,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1991,20 +1974,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2017,15 +1986,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1047750</xdr:colOff>
+          <xdr:colOff>1054100</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>866775</xdr:colOff>
+          <xdr:colOff>863600</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2038,7 +2007,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2046,20 +2015,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2072,15 +2027,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>25400</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>241300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2093,7 +2048,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2101,20 +2056,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2129,13 +2070,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2148,7 +2089,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2156,20 +2097,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2182,15 +2109,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1016000</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>828675</xdr:colOff>
+          <xdr:colOff>825500</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2203,7 +2130,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2211,20 +2138,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2237,15 +2150,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2258,7 +2171,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2266,20 +2179,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2292,15 +2191,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>12700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>482600</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>711200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2313,7 +2212,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2321,20 +2220,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2667,34 +2552,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="34.875" style="15" customWidth="1"/>
-    <col min="11" max="11" width="29.625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="20.375" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="34.83203125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="10.875" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.875" style="2"/>
+    <col min="14" max="15" width="10.83203125" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2713,19 +2598,19 @@
         <v xml:space="preserve">Ubicación de la imagen en el recurso </v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="85"/>
-      <c r="F2" s="77" t="s">
+      <c r="D2" s="82"/>
+      <c r="F2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="78"/>
+      <c r="G2" s="75"/>
       <c r="H2" s="58"/>
       <c r="I2" s="58"/>
       <c r="J2" s="14"/>
@@ -2744,19 +2629,19 @@
         <v>M3A</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.75">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="86">
+      <c r="C3" s="83">
         <v>6</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="F3" s="79">
+      <c r="D3" s="84"/>
+      <c r="F3" s="76">
         <v>42458</v>
       </c>
-      <c r="G3" s="80"/>
+      <c r="G3" s="77"/>
       <c r="H3" s="58"/>
       <c r="I3" s="38"/>
       <c r="J3" s="14"/>
@@ -2775,15 +2660,15 @@
         <v>M5A</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="16.5">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="83" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="87"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="5"/>
       <c r="F4" s="37" t="s">
         <v>55</v>
@@ -2807,15 +2692,15 @@
         <v>M6A</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="17.25" thickBot="1">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="88" t="s">
+      <c r="C5" s="85" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="89"/>
+      <c r="D5" s="86"/>
       <c r="E5" s="5"/>
       <c r="F5" s="37" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2838,7 +2723,7 @@
         <v>M7A</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="16.5" thickBot="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2862,12 +2747,12 @@
         <v>M8A</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="70" t="s">
         <v>190</v>
       </c>
       <c r="D7" s="23" t="s">
@@ -2891,18 +2776,18 @@
         <v>M9B</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="8" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" s="8" customFormat="1" ht="16.5" thickBot="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="83"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="80"/>
       <c r="J8" s="16"/>
       <c r="K8" s="11"/>
       <c r="M8" s="2" t="str">
@@ -2918,7 +2803,7 @@
       </c>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="38.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="38.75" customHeight="1" thickBot="1">
       <c r="A9" s="21" t="s">
         <v>2</v>
       </c>
@@ -2958,87 +2843,87 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="str">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="15">
+      <c r="A10" s="106" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
-      <c r="B10" s="108">
+      <c r="B10" s="107">
         <v>32237011</v>
       </c>
-      <c r="C10" s="20" t="str">
+      <c r="C10" s="108" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="F10" s="13" t="str">
+      <c r="F10" s="105" t="str">
         <f t="shared" ref="F10" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>LE_06_08_CO_IMG01_small</v>
       </c>
-      <c r="G10" s="13" t="str">
+      <c r="G10" s="105" t="str">
         <f ca="1">IF($F10&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H10" s="13" t="str">
+      <c r="H10" s="105" t="str">
         <f t="shared" ref="H10" ca="1" si="2">IF(AND(I10&lt;&gt;"",I10&lt;&gt;0),IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>LE_06_08_CO_IMG01_zoom</v>
       </c>
-      <c r="I10" s="13" t="str">
+      <c r="I10" s="105" t="str">
         <f ca="1">IF(OR($B10&lt;&gt;"",$J10&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J10" s="109" t="s">
+      <c r="J10" s="107" t="s">
         <v>192</v>
       </c>
-      <c r="K10" s="64"/>
+      <c r="K10" s="110"/>
       <c r="O10" s="2" t="str">
         <f>'Definición técnica de imagenes'!A12</f>
         <v>M12D</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="11" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="str">
+    <row r="11" spans="1:16" s="11" customFormat="1" ht="72" customHeight="1">
+      <c r="A11" s="106" t="str">
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="108">
+      <c r="B11" s="107">
         <v>163286372</v>
       </c>
-      <c r="C11" s="20" t="str">
+      <c r="C11" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="109" t="s">
         <v>194</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E11" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="F11" s="13" t="str">
+      <c r="F11" s="105" t="str">
         <f t="shared" ref="F11:F74" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>LE_06_08_CO_IMG02_small</v>
       </c>
-      <c r="G11" s="13" t="str">
+      <c r="G11" s="105" t="str">
         <f ca="1">IF($F11&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H11" s="13" t="str">
+      <c r="H11" s="105" t="str">
         <f t="shared" ref="H11:H74" ca="1" si="5">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>LE_06_08_CO_IMG02_zoom</v>
       </c>
-      <c r="I11" s="13" t="str">
+      <c r="I11" s="105" t="str">
         <f ca="1">IF(OR($B11&lt;&gt;"",$J11&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J11" s="110" t="s">
+      <c r="J11" s="107" t="s">
         <v>193</v>
       </c>
-      <c r="K11" s="65" t="s">
+      <c r="K11" s="110" t="s">
         <v>196</v>
       </c>
       <c r="O11" s="2" t="str">
@@ -3046,44 +2931,44 @@
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="str">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="58" customHeight="1">
+      <c r="A12" s="106" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="108">
+      <c r="B12" s="107">
         <v>179128526</v>
       </c>
-      <c r="C12" s="20" t="str">
+      <c r="C12" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="109" t="s">
         <v>194</v>
       </c>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="F12" s="13" t="str">
+      <c r="F12" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG03_small</v>
       </c>
-      <c r="G12" s="13" t="str">
+      <c r="G12" s="105" t="str">
         <f ca="1">IF($F12&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H12" s="13" t="str">
+      <c r="H12" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG03_zoom</v>
       </c>
-      <c r="I12" s="13" t="str">
+      <c r="I12" s="105" t="str">
         <f ca="1">IF(OR($B12&lt;&gt;"",$J12&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12" s="110" t="s">
+      <c r="J12" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="K12" s="64" t="s">
+      <c r="K12" s="110" t="s">
         <v>197</v>
       </c>
       <c r="O12" s="2" t="str">
@@ -3091,87 +2976,87 @@
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="str">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="15">
+      <c r="A13" s="106" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
       <c r="B13" s="111">
         <v>68876089</v>
       </c>
-      <c r="C13" s="20" t="str">
+      <c r="C13" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="E13" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="F13" s="13" t="str">
+      <c r="F13" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG04_small</v>
       </c>
-      <c r="G13" s="13" t="str">
+      <c r="G13" s="105" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H13" s="13" t="str">
+      <c r="H13" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG04_zoom</v>
       </c>
-      <c r="I13" s="13" t="str">
+      <c r="I13" s="105" t="str">
         <f ca="1">IF(OR($B13&lt;&gt;"",$J13&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J13" s="110" t="s">
+      <c r="J13" s="107" t="s">
         <v>198</v>
       </c>
-      <c r="K13" s="64"/>
+      <c r="K13" s="110"/>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="str">
+    <row r="14" spans="1:16" s="11" customFormat="1" ht="135" customHeight="1">
+      <c r="A14" s="106" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
       </c>
-      <c r="B14" s="109" t="s">
+      <c r="B14" s="107" t="s">
         <v>199</v>
       </c>
-      <c r="C14" s="20" t="str">
+      <c r="C14" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E14" s="63" t="s">
+      <c r="E14" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="F14" s="13" t="str">
+      <c r="F14" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG05_small</v>
       </c>
-      <c r="G14" s="13" t="str">
+      <c r="G14" s="105" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H14" s="13" t="str">
+      <c r="H14" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG05_zoom</v>
       </c>
-      <c r="I14" s="13" t="str">
+      <c r="I14" s="105" t="str">
         <f ca="1">IF(OR($B14&lt;&gt;"",$J14&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J14" s="110" t="s">
+      <c r="J14" s="107" t="s">
         <v>200</v>
       </c>
-      <c r="K14" s="64" t="s">
+      <c r="K14" s="110" t="s">
         <v>210</v>
       </c>
       <c r="O14" s="2" t="str">
@@ -3179,394 +3064,394 @@
         <v>F6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="str">
+    <row r="15" spans="1:16" s="11" customFormat="1" ht="15">
+      <c r="A15" s="106" t="str">
         <f t="shared" si="3"/>
         <v>IMG06</v>
       </c>
       <c r="B15" s="111">
         <v>378757225</v>
       </c>
-      <c r="C15" s="20" t="str">
+      <c r="C15" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="F15" s="13" t="str">
+      <c r="F15" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG06_small</v>
       </c>
-      <c r="G15" s="13" t="str">
+      <c r="G15" s="105" t="str">
         <f ca="1">IF($F15&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H15" s="13" t="str">
+      <c r="H15" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG06_zoom</v>
       </c>
-      <c r="I15" s="13" t="str">
+      <c r="I15" s="105" t="str">
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J15" s="110" t="s">
+      <c r="J15" s="107" t="s">
         <v>201</v>
       </c>
-      <c r="K15" s="66"/>
+      <c r="K15" s="110"/>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="str">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="15">
+      <c r="A16" s="106" t="str">
         <f t="shared" si="3"/>
         <v>IMG07</v>
       </c>
-      <c r="B16" s="112">
+      <c r="B16" s="107">
         <v>79196662</v>
       </c>
-      <c r="C16" s="20" t="str">
+      <c r="C16" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D16" s="63" t="s">
+      <c r="D16" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="E16" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="F16" s="13" t="str">
+      <c r="F16" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG07_small</v>
       </c>
-      <c r="G16" s="13" t="str">
+      <c r="G16" s="105" t="str">
         <f ca="1">IF($F16&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H16" s="13" t="str">
+      <c r="H16" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG07_zoom</v>
       </c>
-      <c r="I16" s="13" t="str">
+      <c r="I16" s="105" t="str">
         <f ca="1">IF(OR($B16&lt;&gt;"",$J16&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J16" s="110" t="s">
+      <c r="J16" s="107" t="s">
         <v>202</v>
       </c>
-      <c r="K16" s="67"/>
+      <c r="K16" s="110"/>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
         <v>F7</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="str">
+    <row r="17" spans="1:15" s="11" customFormat="1" ht="15">
+      <c r="A17" s="106" t="str">
         <f t="shared" si="3"/>
         <v>IMG08</v>
       </c>
-      <c r="B17" s="112">
+      <c r="B17" s="107">
         <v>324217466</v>
       </c>
-      <c r="C17" s="20" t="str">
+      <c r="C17" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="F17" s="13" t="str">
+      <c r="F17" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG08_small</v>
       </c>
-      <c r="G17" s="13" t="str">
+      <c r="G17" s="105" t="str">
         <f ca="1">IF($F17&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H17" s="13" t="str">
+      <c r="H17" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG08_zoom</v>
       </c>
-      <c r="I17" s="13" t="str">
+      <c r="I17" s="105" t="str">
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J17" s="110" t="s">
+      <c r="J17" s="107" t="s">
         <v>203</v>
       </c>
-      <c r="K17" s="66"/>
+      <c r="K17" s="110"/>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
         <v>F7B</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="str">
+    <row r="18" spans="1:15" s="11" customFormat="1" ht="16" thickBot="1">
+      <c r="A18" s="106" t="str">
         <f t="shared" si="3"/>
         <v>IMG09</v>
       </c>
-      <c r="B18" s="108">
+      <c r="B18" s="107">
         <v>129162242</v>
       </c>
-      <c r="C18" s="20" t="str">
+      <c r="C18" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E18" s="63" t="s">
+      <c r="E18" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="F18" s="13" t="str">
+      <c r="F18" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG09_small</v>
       </c>
-      <c r="G18" s="13" t="str">
+      <c r="G18" s="105" t="str">
         <f ca="1">IF($F18&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H18" s="13" t="str">
+      <c r="H18" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG09_zoom</v>
       </c>
-      <c r="I18" s="13" t="str">
+      <c r="I18" s="105" t="str">
         <f ca="1">IF(OR($B18&lt;&gt;"",$J18&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J18" s="109" t="s">
+      <c r="J18" s="107" t="s">
         <v>204</v>
       </c>
-      <c r="K18" s="66"/>
+      <c r="K18" s="110"/>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
         <v>F8</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="11" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="str">
+    <row r="19" spans="1:15" s="11" customFormat="1" ht="16" thickBot="1">
+      <c r="A19" s="106" t="str">
         <f t="shared" ref="A19:A50" si="6">IF(OR(B19&lt;&gt;"",J19&lt;&gt;""),CONCATENATE(LEFT(A18,3),IF(MID(A18,4,2)+1&lt;10,CONCATENATE("0",MID(A18,4,2)+1),MID(A18,4,2)+1)),"")</f>
         <v>IMG10</v>
       </c>
-      <c r="B19" s="113">
+      <c r="B19" s="112">
         <v>295915793</v>
       </c>
-      <c r="C19" s="20" t="str">
+      <c r="C19" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D19" s="63" t="s">
+      <c r="D19" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E19" s="63" t="s">
+      <c r="E19" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="F19" s="13" t="str">
+      <c r="F19" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG10_small</v>
       </c>
-      <c r="G19" s="13" t="str">
+      <c r="G19" s="105" t="str">
         <f ca="1">IF($F19&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H19" s="13" t="str">
+      <c r="H19" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG10_zoom</v>
       </c>
-      <c r="I19" s="13" t="str">
+      <c r="I19" s="105" t="str">
         <f ca="1">IF(OR($B19&lt;&gt;"",$J19&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J19" s="110" t="s">
+      <c r="J19" s="107" t="s">
         <v>205</v>
       </c>
-      <c r="K19" s="67"/>
+      <c r="K19" s="110"/>
       <c r="O19" s="2" t="str">
         <f>'Definición técnica de imagenes'!A31</f>
         <v>F10</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="str">
+    <row r="20" spans="1:15" s="11" customFormat="1" ht="15">
+      <c r="A20" s="106" t="str">
         <f t="shared" si="6"/>
         <v>IMG11</v>
       </c>
-      <c r="B20" s="108">
+      <c r="B20" s="107">
         <v>129391076</v>
       </c>
-      <c r="C20" s="20" t="str">
+      <c r="C20" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D20" s="63" t="s">
+      <c r="D20" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E20" s="63" t="s">
+      <c r="E20" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="F20" s="13" t="str">
+      <c r="F20" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG11_small</v>
       </c>
-      <c r="G20" s="13" t="str">
+      <c r="G20" s="105" t="str">
         <f ca="1">IF($F20&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H20" s="13" t="str">
+      <c r="H20" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG11_zoom</v>
       </c>
-      <c r="I20" s="13" t="str">
+      <c r="I20" s="105" t="str">
         <f ca="1">IF(OR($B20&lt;&gt;"",$J20&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J20" s="110" t="s">
+      <c r="J20" s="107" t="s">
         <v>206</v>
       </c>
-      <c r="K20" s="66"/>
+      <c r="K20" s="110"/>
       <c r="O20" s="2" t="str">
         <f>'Definición técnica de imagenes'!A32</f>
         <v>F10B</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="str">
+    <row r="21" spans="1:15" s="11" customFormat="1" ht="15">
+      <c r="A21" s="106" t="str">
         <f t="shared" si="6"/>
         <v>IMG12</v>
       </c>
       <c r="B21" s="111">
         <v>313789634</v>
       </c>
-      <c r="C21" s="20" t="str">
+      <c r="C21" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D21" s="63" t="s">
+      <c r="D21" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E21" s="63" t="s">
+      <c r="E21" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="F21" s="13" t="str">
+      <c r="F21" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG12_small</v>
       </c>
-      <c r="G21" s="13" t="str">
+      <c r="G21" s="105" t="str">
         <f ca="1">IF($F21&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H21" s="13" t="str">
+      <c r="H21" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG12_zoom</v>
       </c>
-      <c r="I21" s="13" t="str">
+      <c r="I21" s="105" t="str">
         <f ca="1">IF(OR($B21&lt;&gt;"",$J21&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J21" s="110" t="s">
+      <c r="J21" s="107" t="s">
         <v>207</v>
       </c>
-      <c r="K21" s="66"/>
+      <c r="K21" s="110"/>
       <c r="O21" s="2" t="str">
         <f>'Definición técnica de imagenes'!A33</f>
         <v>F11</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="str">
+    <row r="22" spans="1:15" s="11" customFormat="1" ht="15">
+      <c r="A22" s="106" t="str">
         <f t="shared" si="6"/>
         <v>IMG13</v>
       </c>
-      <c r="B22" s="108">
+      <c r="B22" s="107">
         <v>293854103</v>
       </c>
-      <c r="C22" s="20" t="str">
+      <c r="C22" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D22" s="63" t="s">
+      <c r="D22" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E22" s="63" t="s">
+      <c r="E22" s="109" t="s">
         <v>154</v>
       </c>
-      <c r="F22" s="13" t="str">
+      <c r="F22" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG13_small</v>
       </c>
-      <c r="G22" s="13" t="str">
+      <c r="G22" s="105" t="str">
         <f ca="1">IF($F22&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E22,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H22" s="13" t="str">
+      <c r="H22" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG13_zoom</v>
       </c>
-      <c r="I22" s="13" t="str">
+      <c r="I22" s="105" t="str">
         <f ca="1">IF(OR($B22&lt;&gt;"",$J22&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E22,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E22,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J22" s="110" t="s">
+      <c r="J22" s="107" t="s">
         <v>208</v>
       </c>
-      <c r="K22" s="68"/>
+      <c r="K22" s="109"/>
       <c r="O22" s="2" t="str">
         <f>'Definición técnica de imagenes'!A34</f>
         <v>F12</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="str">
+    <row r="23" spans="1:15" s="11" customFormat="1" ht="15">
+      <c r="A23" s="106" t="str">
         <f t="shared" si="6"/>
         <v>IMG14</v>
       </c>
       <c r="B23" s="111">
         <v>313996466</v>
       </c>
-      <c r="C23" s="20" t="str">
+      <c r="C23" s="108" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D23" s="63" t="s">
+      <c r="D23" s="109" t="s">
         <v>191</v>
       </c>
-      <c r="E23" s="63" t="s">
+      <c r="E23" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="F23" s="13" t="str">
+      <c r="F23" s="105" t="str">
         <f t="shared" si="4"/>
         <v>LE_06_08_CO_IMG14_small</v>
       </c>
-      <c r="G23" s="13" t="str">
+      <c r="G23" s="105" t="str">
         <f ca="1">IF($F23&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E23,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>526 x 370 px</v>
       </c>
-      <c r="H23" s="13" t="str">
+      <c r="H23" s="105" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>LE_06_08_CO_IMG14_zoom</v>
       </c>
-      <c r="I23" s="13" t="str">
+      <c r="I23" s="105" t="str">
         <f ca="1">IF(OR($B23&lt;&gt;"",$J23&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E23,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E23,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J23" s="109" t="s">
+      <c r="J23" s="107" t="s">
         <v>209</v>
       </c>
-      <c r="K23" s="64"/>
+      <c r="K23" s="110"/>
       <c r="O23" s="2" t="str">
         <f>'Definición técnica de imagenes'!A35</f>
         <v>F13</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A24" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3601,7 +3486,7 @@
         <v>F13B</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A25" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3632,7 +3517,7 @@
       <c r="J25" s="63"/>
       <c r="K25" s="64"/>
     </row>
-    <row r="26" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A26" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3663,7 +3548,7 @@
       <c r="J26" s="63"/>
       <c r="K26" s="64"/>
     </row>
-    <row r="27" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A27" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3695,7 +3580,7 @@
       <c r="K27" s="64"/>
       <c r="O27" s="2"/>
     </row>
-    <row r="28" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A28" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3726,7 +3611,7 @@
       <c r="J28" s="64"/>
       <c r="K28" s="64"/>
     </row>
-    <row r="29" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A29" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3757,7 +3642,7 @@
       <c r="J29" s="64"/>
       <c r="K29" s="64"/>
     </row>
-    <row r="30" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A30" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3788,7 +3673,7 @@
       <c r="J30" s="64"/>
       <c r="K30" s="64"/>
     </row>
-    <row r="31" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A31" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3819,7 +3704,7 @@
       <c r="J31" s="64"/>
       <c r="K31" s="64"/>
     </row>
-    <row r="32" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A32" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3850,7 +3735,7 @@
       <c r="J32" s="64"/>
       <c r="K32" s="64"/>
     </row>
-    <row r="33" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A33" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3881,7 +3766,7 @@
       <c r="J33" s="64"/>
       <c r="K33" s="64"/>
     </row>
-    <row r="34" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A34" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3913,7 +3798,7 @@
       <c r="K34" s="64"/>
       <c r="O34" s="2"/>
     </row>
-    <row r="35" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A35" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3945,7 +3830,7 @@
       <c r="K35" s="65"/>
       <c r="O35" s="2"/>
     </row>
-    <row r="36" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A36" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3977,7 +3862,7 @@
       <c r="K36" s="65"/>
       <c r="O36" s="2"/>
     </row>
-    <row r="37" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A37" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4005,10 +3890,10 @@
         <f ca="1">IF(OR($B37&lt;&gt;"",$J37&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E37,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E37,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J37" s="69"/>
+      <c r="J37" s="66"/>
       <c r="K37" s="65"/>
     </row>
-    <row r="38" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A38" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4036,10 +3921,10 @@
         <f ca="1">IF(OR($B38&lt;&gt;"",$J38&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E38,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E38,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v/>
       </c>
-      <c r="J38" s="70"/>
+      <c r="J38" s="67"/>
       <c r="K38" s="65"/>
     </row>
-    <row r="39" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A39" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4070,7 +3955,7 @@
       <c r="J39" s="63"/>
       <c r="K39" s="65"/>
     </row>
-    <row r="40" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A40" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4101,7 +3986,7 @@
       <c r="J40" s="63"/>
       <c r="K40" s="65"/>
     </row>
-    <row r="41" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A41" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4132,7 +4017,7 @@
       <c r="J41" s="63"/>
       <c r="K41" s="65"/>
     </row>
-    <row r="42" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A42" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4163,7 +4048,7 @@
       <c r="J42" s="63"/>
       <c r="K42" s="65"/>
     </row>
-    <row r="43" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A43" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4194,7 +4079,7 @@
       <c r="J43" s="63"/>
       <c r="K43" s="65"/>
     </row>
-    <row r="44" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A44" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4225,7 +4110,7 @@
       <c r="J44" s="63"/>
       <c r="K44" s="65"/>
     </row>
-    <row r="45" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A45" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4256,7 +4141,7 @@
       <c r="J45" s="63"/>
       <c r="K45" s="65"/>
     </row>
-    <row r="46" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A46" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4287,7 +4172,7 @@
       <c r="J46" s="63"/>
       <c r="K46" s="65"/>
     </row>
-    <row r="47" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A47" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4318,7 +4203,7 @@
       <c r="J47" s="63"/>
       <c r="K47" s="65"/>
     </row>
-    <row r="48" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" s="11" customFormat="1" ht="15">
       <c r="A48" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4349,7 +4234,7 @@
       <c r="J48" s="63"/>
       <c r="K48" s="65"/>
     </row>
-    <row r="49" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A49" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4380,7 +4265,7 @@
       <c r="J49" s="63"/>
       <c r="K49" s="65"/>
     </row>
-    <row r="50" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A50" s="12" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -4411,7 +4296,7 @@
       <c r="J50" s="63"/>
       <c r="K50" s="65"/>
     </row>
-    <row r="51" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A51" s="12" t="str">
         <f t="shared" ref="A51:A82" si="8">IF(OR(B51&lt;&gt;"",J51&lt;&gt;""),CONCATENATE(LEFT(A50,3),IF(MID(A50,4,2)+1&lt;10,CONCATENATE("0",MID(A50,4,2)+1),MID(A50,4,2)+1)),"")</f>
         <v/>
@@ -4442,7 +4327,7 @@
       <c r="J51" s="63"/>
       <c r="K51" s="65"/>
     </row>
-    <row r="52" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A52" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4473,7 +4358,7 @@
       <c r="J52" s="63"/>
       <c r="K52" s="65"/>
     </row>
-    <row r="53" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A53" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4504,7 +4389,7 @@
       <c r="J53" s="63"/>
       <c r="K53" s="65"/>
     </row>
-    <row r="54" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A54" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4535,7 +4420,7 @@
       <c r="J54" s="63"/>
       <c r="K54" s="65"/>
     </row>
-    <row r="55" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A55" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4566,7 +4451,7 @@
       <c r="J55" s="63"/>
       <c r="K55" s="65"/>
     </row>
-    <row r="56" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A56" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4597,7 +4482,7 @@
       <c r="J56" s="63"/>
       <c r="K56" s="65"/>
     </row>
-    <row r="57" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A57" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4628,7 +4513,7 @@
       <c r="J57" s="63"/>
       <c r="K57" s="65"/>
     </row>
-    <row r="58" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A58" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4659,7 +4544,7 @@
       <c r="J58" s="63"/>
       <c r="K58" s="65"/>
     </row>
-    <row r="59" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A59" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4690,7 +4575,7 @@
       <c r="J59" s="63"/>
       <c r="K59" s="65"/>
     </row>
-    <row r="60" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A60" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4721,7 +4606,7 @@
       <c r="J60" s="63"/>
       <c r="K60" s="65"/>
     </row>
-    <row r="61" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A61" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4752,7 +4637,7 @@
       <c r="J61" s="63"/>
       <c r="K61" s="65"/>
     </row>
-    <row r="62" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A62" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4783,7 +4668,7 @@
       <c r="J62" s="63"/>
       <c r="K62" s="65"/>
     </row>
-    <row r="63" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A63" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4814,7 +4699,7 @@
       <c r="J63" s="63"/>
       <c r="K63" s="65"/>
     </row>
-    <row r="64" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A64" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4845,7 +4730,7 @@
       <c r="J64" s="63"/>
       <c r="K64" s="65"/>
     </row>
-    <row r="65" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A65" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4876,7 +4761,7 @@
       <c r="J65" s="63"/>
       <c r="K65" s="65"/>
     </row>
-    <row r="66" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A66" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4907,7 +4792,7 @@
       <c r="J66" s="63"/>
       <c r="K66" s="65"/>
     </row>
-    <row r="67" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A67" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4938,7 +4823,7 @@
       <c r="J67" s="63"/>
       <c r="K67" s="65"/>
     </row>
-    <row r="68" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A68" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4969,7 +4854,7 @@
       <c r="J68" s="63"/>
       <c r="K68" s="65"/>
     </row>
-    <row r="69" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A69" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5000,7 +4885,7 @@
       <c r="J69" s="63"/>
       <c r="K69" s="65"/>
     </row>
-    <row r="70" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A70" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5031,7 +4916,7 @@
       <c r="J70" s="63"/>
       <c r="K70" s="65"/>
     </row>
-    <row r="71" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A71" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5062,7 +4947,7 @@
       <c r="J71" s="63"/>
       <c r="K71" s="65"/>
     </row>
-    <row r="72" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A72" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5093,7 +4978,7 @@
       <c r="J72" s="63"/>
       <c r="K72" s="65"/>
     </row>
-    <row r="73" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A73" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5124,7 +5009,7 @@
       <c r="J73" s="63"/>
       <c r="K73" s="65"/>
     </row>
-    <row r="74" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A74" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5155,7 +5040,7 @@
       <c r="J74" s="63"/>
       <c r="K74" s="65"/>
     </row>
-    <row r="75" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A75" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5186,7 +5071,7 @@
       <c r="J75" s="63"/>
       <c r="K75" s="65"/>
     </row>
-    <row r="76" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A76" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5217,7 +5102,7 @@
       <c r="J76" s="63"/>
       <c r="K76" s="65"/>
     </row>
-    <row r="77" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A77" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5248,7 +5133,7 @@
       <c r="J77" s="63"/>
       <c r="K77" s="65"/>
     </row>
-    <row r="78" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A78" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5279,7 +5164,7 @@
       <c r="J78" s="63"/>
       <c r="K78" s="65"/>
     </row>
-    <row r="79" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A79" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5310,7 +5195,7 @@
       <c r="J79" s="63"/>
       <c r="K79" s="65"/>
     </row>
-    <row r="80" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A80" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5341,7 +5226,7 @@
       <c r="J80" s="63"/>
       <c r="K80" s="65"/>
     </row>
-    <row r="81" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A81" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5372,7 +5257,7 @@
       <c r="J81" s="63"/>
       <c r="K81" s="65"/>
     </row>
-    <row r="82" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A82" s="12" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -5403,7 +5288,7 @@
       <c r="J82" s="63"/>
       <c r="K82" s="65"/>
     </row>
-    <row r="83" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A83" s="12" t="str">
         <f t="shared" ref="A83:A108" si="12">IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),CONCATENATE(LEFT(A82,3),IF(MID(A82,4,2)+1&lt;10,CONCATENATE("0",MID(A82,4,2)+1),MID(A82,4,2)+1)),"")</f>
         <v/>
@@ -5434,7 +5319,7 @@
       <c r="J83" s="63"/>
       <c r="K83" s="65"/>
     </row>
-    <row r="84" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A84" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5465,7 +5350,7 @@
       <c r="J84" s="63"/>
       <c r="K84" s="65"/>
     </row>
-    <row r="85" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A85" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5496,7 +5381,7 @@
       <c r="J85" s="63"/>
       <c r="K85" s="65"/>
     </row>
-    <row r="86" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A86" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5527,7 +5412,7 @@
       <c r="J86" s="63"/>
       <c r="K86" s="65"/>
     </row>
-    <row r="87" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A87" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5558,7 +5443,7 @@
       <c r="J87" s="63"/>
       <c r="K87" s="65"/>
     </row>
-    <row r="88" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A88" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5589,7 +5474,7 @@
       <c r="J88" s="63"/>
       <c r="K88" s="65"/>
     </row>
-    <row r="89" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A89" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5620,7 +5505,7 @@
       <c r="J89" s="63"/>
       <c r="K89" s="65"/>
     </row>
-    <row r="90" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A90" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5651,7 +5536,7 @@
       <c r="J90" s="63"/>
       <c r="K90" s="65"/>
     </row>
-    <row r="91" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A91" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5682,7 +5567,7 @@
       <c r="J91" s="63"/>
       <c r="K91" s="65"/>
     </row>
-    <row r="92" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A92" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5713,7 +5598,7 @@
       <c r="J92" s="63"/>
       <c r="K92" s="65"/>
     </row>
-    <row r="93" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A93" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5744,7 +5629,7 @@
       <c r="J93" s="63"/>
       <c r="K93" s="65"/>
     </row>
-    <row r="94" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A94" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5775,7 +5660,7 @@
       <c r="J94" s="63"/>
       <c r="K94" s="65"/>
     </row>
-    <row r="95" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A95" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5806,7 +5691,7 @@
       <c r="J95" s="63"/>
       <c r="K95" s="65"/>
     </row>
-    <row r="96" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A96" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5837,7 +5722,7 @@
       <c r="J96" s="63"/>
       <c r="K96" s="65"/>
     </row>
-    <row r="97" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A97" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5868,7 +5753,7 @@
       <c r="J97" s="63"/>
       <c r="K97" s="65"/>
     </row>
-    <row r="98" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A98" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5899,7 +5784,7 @@
       <c r="J98" s="63"/>
       <c r="K98" s="65"/>
     </row>
-    <row r="99" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A99" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5930,7 +5815,7 @@
       <c r="J99" s="63"/>
       <c r="K99" s="65"/>
     </row>
-    <row r="100" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A100" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5961,7 +5846,7 @@
       <c r="J100" s="63"/>
       <c r="K100" s="65"/>
     </row>
-    <row r="101" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A101" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -5992,7 +5877,7 @@
       <c r="J101" s="63"/>
       <c r="K101" s="65"/>
     </row>
-    <row r="102" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A102" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6023,7 +5908,7 @@
       <c r="J102" s="63"/>
       <c r="K102" s="65"/>
     </row>
-    <row r="103" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A103" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6054,7 +5939,7 @@
       <c r="J103" s="63"/>
       <c r="K103" s="65"/>
     </row>
-    <row r="104" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A104" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6085,7 +5970,7 @@
       <c r="J104" s="63"/>
       <c r="K104" s="65"/>
     </row>
-    <row r="105" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A105" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6116,7 +6001,7 @@
       <c r="J105" s="63"/>
       <c r="K105" s="65"/>
     </row>
-    <row r="106" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A106" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6147,7 +6032,7 @@
       <c r="J106" s="63"/>
       <c r="K106" s="65"/>
     </row>
-    <row r="107" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A107" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6178,7 +6063,7 @@
       <c r="J107" s="63"/>
       <c r="K107" s="65"/>
     </row>
-    <row r="108" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" s="11" customFormat="1" ht="15">
       <c r="A108" s="12" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -6210,7 +6095,7 @@
       <c r="K108" s="65"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="77H5Iqzv9dZcGmmBaf69JMJb19F7NL/TII5UwBSFOuUaqVrFbpC0VyStjTSM9GXqoLW1eBJcnDtnuP0mFWowpA==" saltValue="GBL6OckecvWR/Pgb/M/1sg==" spinCount="100000" sheet="1" scenarios="1" formatColumns="0" formatRows="0" selectLockedCells="1"/>
+  <sheetProtection formatColumns="0" formatRows="0" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -6263,63 +6148,68 @@
     <hyperlink ref="B23" r:id="rId11" display="http://www.shutterstock.com/pic.mhtml?id=313996466&amp;src=id"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId12"/>
-  <drawing r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId12"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2"/>
+  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="72.25" style="22" customWidth="1"/>
-    <col min="2" max="2" width="11" style="22"/>
-    <col min="3" max="3" width="13.875" style="22" customWidth="1"/>
-    <col min="4" max="4" width="11.375" style="22" customWidth="1"/>
-    <col min="5" max="7" width="11" style="22"/>
+    <col min="1" max="1" width="72.1640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="22"/>
+    <col min="3" max="3" width="13.83203125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="22" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="22"/>
     <col min="8" max="11" width="11" style="22" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="22"/>
+    <col min="12" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="92" t="s">
+    <row r="1" spans="1:11" ht="16.5" thickBot="1">
+      <c r="A1" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="94"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31"/>
-      <c r="C2" s="95" t="s">
+      <c r="C2" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="63">
       <c r="A3" s="33" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="101" t="s">
+      <c r="C3" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="102"/>
-      <c r="E3" s="103"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="100"/>
       <c r="F3" s="32"/>
       <c r="H3" s="22" t="s">
         <v>18</v>
@@ -6334,7 +6224,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="31.5">
       <c r="A4" s="30" t="s">
         <v>44</v>
       </c>
@@ -6362,7 +6252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="79.5" thickBot="1">
       <c r="A5" s="33" t="s">
         <v>45</v>
       </c>
@@ -6370,11 +6260,11 @@
       <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="104" t="str">
+      <c r="D5" s="101" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="105"/>
+      <c r="E5" s="102"/>
       <c r="F5" s="32"/>
       <c r="H5" s="22" t="s">
         <v>22</v>
@@ -6389,7 +6279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="32.25" thickBot="1">
       <c r="A6" s="30" t="s">
         <v>10</v>
       </c>
@@ -6411,7 +6301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="48" thickBot="1">
       <c r="A7" s="33" t="s">
         <v>11</v>
       </c>
@@ -6419,12 +6309,12 @@
       <c r="C7" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="90" t="str">
+      <c r="D7" s="87" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="90"/>
-      <c r="F7" s="91"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="88"/>
       <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
@@ -6438,7 +6328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="47.25">
       <c r="A8" s="33" t="s">
         <v>53</v>
       </c>
@@ -6457,7 +6347,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="47.25">
       <c r="A9" s="33" t="s">
         <v>12</v>
       </c>
@@ -6476,7 +6366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="32.25" thickBot="1">
       <c r="A10" s="34" t="s">
         <v>36</v>
       </c>
@@ -6495,7 +6385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="I11" s="22" t="s">
         <v>32</v>
       </c>
@@ -6506,7 +6396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="16.5" thickBot="1">
       <c r="I12" s="22" t="s">
         <v>37</v>
       </c>
@@ -6517,15 +6407,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="92" t="s">
+    <row r="13" spans="1:11">
+      <c r="A13" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="94"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="91"/>
       <c r="I13" s="22" t="s">
         <v>33</v>
       </c>
@@ -6536,7 +6426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="16.5" thickBot="1">
       <c r="A14" s="33"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -6553,17 +6443,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="30" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="97"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
+      <c r="F15" s="94"/>
       <c r="J15" s="22">
         <v>12</v>
       </c>
@@ -6571,7 +6461,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="67.25" customHeight="1">
       <c r="A16" s="33" t="s">
         <v>47</v>
       </c>
@@ -6595,7 +6485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="32" customHeight="1" thickBot="1">
       <c r="A17" s="30" t="s">
         <v>44</v>
       </c>
@@ -6603,12 +6493,12 @@
       <c r="C17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="98" t="str">
+      <c r="D17" s="95" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="99"/>
-      <c r="F17" s="100"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="97"/>
       <c r="J17" s="22">
         <v>14</v>
       </c>
@@ -6616,7 +6506,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="79.5" thickBot="1">
       <c r="A18" s="33" t="s">
         <v>48</v>
       </c>
@@ -6624,12 +6514,12 @@
       <c r="C18" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="90" t="str">
+      <c r="D18" s="87" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="90"/>
-      <c r="F18" s="91"/>
+      <c r="E18" s="87"/>
+      <c r="F18" s="88"/>
       <c r="J18" s="22">
         <v>15</v>
       </c>
@@ -6637,7 +6527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="30" t="s">
         <v>10</v>
       </c>
@@ -6656,7 +6546,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1">
       <c r="A20" s="34" t="s">
         <v>51</v>
       </c>
@@ -6678,7 +6568,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="H21" s="22" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -6695,122 +6585,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="K22" s="22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="K23" s="22">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="K24" s="22">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="K25" s="22">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="K26" s="22">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="K27" s="22">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="K28" s="22">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="K29" s="22">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="K30" s="22">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="K31" s="22">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="K32" s="22">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:11">
       <c r="K33" s="22">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:11">
       <c r="K34" s="22">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:11">
       <c r="K35" s="22">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11">
       <c r="K36" s="22">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:11">
       <c r="K37" s="22">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:11">
       <c r="K38" s="22">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:11">
       <c r="K39" s="22">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:11">
       <c r="K40" s="22">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="11:11">
       <c r="K41" s="22">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="11:11">
       <c r="K42" s="22">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="11:11">
       <c r="K43" s="22">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="11:11">
       <c r="K44" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="11:11">
       <c r="K45" s="22" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -6829,169 +6719,181 @@
     <mergeCell ref="D7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId4" name="Drop Down 6">
+            <control shapeId="1030" r:id="rId3" name="Drop Down 6">
               <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId5" name="Drop Down 7">
+            <control shapeId="1031" r:id="rId4" name="Drop Down 7">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1016000</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>828675</xdr:colOff>
+                    <xdr:colOff>825500</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId6" name="Drop Down 8">
+            <control shapeId="1032" r:id="rId5" name="Drop Down 8">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId7" name="Drop Down 11">
+            <control shapeId="1035" r:id="rId6" name="Drop Down 11">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>482600</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>711200</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId8" name="Drop Down 2">
+            <control shapeId="1026" r:id="rId7" name="Drop Down 2">
               <controlPr defaultSize="0" autoLine="0" autoPict="0" macro="[0]!Listadesplegable2_Cambiar">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1038225</xdr:colOff>
+                    <xdr:colOff>1041400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId9" name="Drop Down 4">
+            <control shapeId="1028" r:id="rId8" name="Drop Down 4">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1047750</xdr:colOff>
+                    <xdr:colOff>1054100</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>866775</xdr:colOff>
+                    <xdr:colOff>863600</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId10" name="Drop Down 5">
+            <control shapeId="1029" r:id="rId9" name="Drop Down 5">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>25400</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>12700</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>241300</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
+    <mc:Fallback/>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7004,56 +6906,56 @@
       <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" style="22" customWidth="1"/>
-    <col min="2" max="2" width="24.25" style="22" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="22" customWidth="1"/>
     <col min="3" max="3" width="17" style="22" customWidth="1"/>
-    <col min="4" max="4" width="12.75" style="22" customWidth="1"/>
-    <col min="5" max="5" width="6.875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="12.875" style="22" customWidth="1"/>
-    <col min="7" max="7" width="12.75" style="22" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" style="22" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="22" customWidth="1"/>
     <col min="8" max="8" width="24.5" style="22" customWidth="1"/>
-    <col min="9" max="9" width="27.25" style="22" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" style="22" customWidth="1"/>
     <col min="10" max="10" width="44.5" style="22" customWidth="1"/>
-    <col min="11" max="16384" width="10.875" style="22"/>
+    <col min="11" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="104" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="107" t="s">
+      <c r="B1" s="104" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="107" t="s">
+      <c r="D1" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="107" t="s">
+      <c r="E1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="107" t="s">
+      <c r="F1" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="107" t="s">
+      <c r="G1" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="106" t="s">
+      <c r="H1" s="103" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="106"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="107"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
+      <c r="I1" s="103"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="104"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
       <c r="H2" s="39" t="s">
         <v>65</v>
       </c>
@@ -7061,7 +6963,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A3" s="40" t="s">
         <v>69</v>
       </c>
@@ -7086,7 +6988,7 @@
       </c>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A4" s="42" t="s">
         <v>57</v>
       </c>
@@ -7115,7 +7017,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A5" s="43" t="s">
         <v>77</v>
       </c>
@@ -7144,7 +7046,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A6" s="42" t="s">
         <v>58</v>
       </c>
@@ -7173,7 +7075,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A7" s="42" t="s">
         <v>58</v>
       </c>
@@ -7198,7 +7100,7 @@
       </c>
       <c r="I7" s="42"/>
     </row>
-    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A8" s="42" t="s">
         <v>80</v>
       </c>
@@ -7227,7 +7129,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A9" s="42" t="s">
         <v>82</v>
       </c>
@@ -7256,7 +7158,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A10" s="42" t="s">
         <v>84</v>
       </c>
@@ -7285,7 +7187,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A11" s="42" t="s">
         <v>86</v>
       </c>
@@ -7310,14 +7212,14 @@
       </c>
       <c r="I11" s="42"/>
     </row>
-    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A12" s="42" t="s">
         <v>89</v>
       </c>
       <c r="B12" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="C12" s="72" t="s">
+      <c r="C12" s="69" t="s">
         <v>90</v>
       </c>
       <c r="D12" s="42" t="s">
@@ -7339,7 +7241,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="41" customFormat="1" ht="14.75" customHeight="1">
       <c r="A13" s="42" t="s">
         <v>91</v>
       </c>
@@ -7368,7 +7270,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="14.75" customHeight="1">
       <c r="A14" s="44" t="s">
         <v>94</v>
       </c>
@@ -7391,33 +7293,33 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="76" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="s">
+    <row r="15" spans="1:10" s="73" customFormat="1" ht="14.75" customHeight="1">
+      <c r="A15" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74" t="s">
+      <c r="B15" s="71"/>
+      <c r="C15" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="74" t="s">
+      <c r="F15" s="71" t="s">
         <v>117</v>
       </c>
-      <c r="G15" s="74"/>
-      <c r="H15" s="75" t="s">
+      <c r="G15" s="71"/>
+      <c r="H15" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="I15" s="74"/>
-      <c r="J15" s="76" t="s">
+      <c r="I15" s="71"/>
+      <c r="J15" s="73" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="14.75" customHeight="1">
       <c r="A16" s="46" t="s">
         <v>100</v>
       </c>
@@ -7445,7 +7347,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="14.75" customHeight="1">
       <c r="A17" s="42" t="s">
         <v>103</v>
       </c>
@@ -7473,7 +7375,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="14.75" customHeight="1">
       <c r="A18" s="42" t="s">
         <v>184</v>
       </c>
@@ -7499,7 +7401,7 @@
       <c r="I18" s="44"/>
       <c r="J18" s="49"/>
     </row>
-    <row r="19" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="14.75" customHeight="1">
       <c r="A19" s="42" t="s">
         <v>137</v>
       </c>
@@ -7523,7 +7425,7 @@
       <c r="I19" s="44"/>
       <c r="J19" s="49"/>
     </row>
-    <row r="20" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="14.75" customHeight="1">
       <c r="A20" s="42" t="s">
         <v>137</v>
       </c>
@@ -7547,7 +7449,7 @@
       <c r="I20" s="44"/>
       <c r="J20" s="49"/>
     </row>
-    <row r="21" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="14.75" customHeight="1">
       <c r="A21" s="42" t="s">
         <v>137</v>
       </c>
@@ -7568,10 +7470,10 @@
       <c r="H21" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="I21" s="71"/>
+      <c r="I21" s="68"/>
       <c r="J21" s="49"/>
     </row>
-    <row r="22" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="14.75" customHeight="1">
       <c r="A22" s="44" t="s">
         <v>132</v>
       </c>
@@ -7595,7 +7497,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="14.75" customHeight="1">
       <c r="A23" s="42" t="s">
         <v>132</v>
       </c>
@@ -7624,7 +7526,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="14.75" customHeight="1">
       <c r="A24" s="42" t="s">
         <v>134</v>
       </c>
@@ -7645,9 +7547,9 @@
         <v>176</v>
       </c>
       <c r="H24" s="44"/>
-      <c r="I24" s="71"/>
-    </row>
-    <row r="25" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="68"/>
+    </row>
+    <row r="25" spans="1:10" ht="14.75" customHeight="1">
       <c r="A25" s="42" t="s">
         <v>135</v>
       </c>
@@ -7671,7 +7573,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="14.75" customHeight="1">
       <c r="A26" s="42" t="s">
         <v>135</v>
       </c>
@@ -7700,7 +7602,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="14.75" customHeight="1">
       <c r="A27" s="42" t="s">
         <v>138</v>
       </c>
@@ -7724,7 +7626,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="14.75" customHeight="1">
       <c r="A28" s="42" t="s">
         <v>138</v>
       </c>
@@ -7748,7 +7650,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="14.75" customHeight="1">
       <c r="A29" s="42" t="s">
         <v>138</v>
       </c>
@@ -7777,7 +7679,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="14.75" customHeight="1">
       <c r="A30" s="42" t="s">
         <v>139</v>
       </c>
@@ -7800,7 +7702,7 @@
       <c r="H30" s="44"/>
       <c r="I30" s="44"/>
     </row>
-    <row r="31" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="14.75" customHeight="1">
       <c r="A31" s="42" t="s">
         <v>140</v>
       </c>
@@ -7817,7 +7719,7 @@
       <c r="H31" s="44"/>
       <c r="I31" s="44"/>
     </row>
-    <row r="32" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="14.75" customHeight="1">
       <c r="A32" s="42" t="s">
         <v>141</v>
       </c>
@@ -7832,7 +7734,7 @@
       <c r="H32" s="44"/>
       <c r="I32" s="44"/>
     </row>
-    <row r="33" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="14.75" customHeight="1">
       <c r="A33" s="42" t="s">
         <v>136</v>
       </c>
@@ -7853,7 +7755,7 @@
       <c r="H33" s="44"/>
       <c r="I33" s="44"/>
     </row>
-    <row r="34" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="14.75" customHeight="1">
       <c r="A34" s="42" t="s">
         <v>142</v>
       </c>
@@ -7870,7 +7772,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="44"/>
     </row>
-    <row r="35" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="14.75" customHeight="1">
       <c r="A35" s="42" t="s">
         <v>95</v>
       </c>
@@ -7899,7 +7801,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="14.75" customHeight="1">
       <c r="A36" s="42" t="s">
         <v>95</v>
       </c>
@@ -7928,7 +7830,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="14.75" customHeight="1">
       <c r="A37" s="42" t="s">
         <v>143</v>
       </c>
@@ -7951,7 +7853,7 @@
       <c r="H37" s="44"/>
       <c r="I37" s="44"/>
     </row>
-    <row r="38" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="14.75" customHeight="1">
       <c r="A38" s="42" t="s">
         <v>143</v>
       </c>
@@ -7974,13 +7876,13 @@
       <c r="H38" s="44"/>
       <c r="I38" s="44"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="50" t="s">
         <v>107</v>
       </c>
       <c r="B40" s="50"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="51" t="s">
         <v>108</v>
       </c>
@@ -7994,7 +7896,7 @@
       <c r="E41" s="52"/>
       <c r="F41" s="52"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="54" t="s">
         <v>109</v>
       </c>
@@ -8008,7 +7910,7 @@
       <c r="E42" s="55"/>
       <c r="F42" s="55"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="54" t="s">
         <v>110</v>
       </c>
@@ -8022,7 +7924,7 @@
       <c r="E43" s="55"/>
       <c r="F43" s="55"/>
     </row>
-    <row r="44" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="31.5">
       <c r="A44" s="54" t="s">
         <v>111</v>
       </c>
@@ -8036,7 +7938,7 @@
       <c r="E44" s="55"/>
       <c r="F44" s="55"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" s="54" t="s">
         <v>112</v>
       </c>
@@ -8050,7 +7952,7 @@
       <c r="E45" s="55"/>
       <c r="F45" s="55"/>
     </row>
-    <row r="46" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="47.25">
       <c r="A46" s="54" t="s">
         <v>162</v>
       </c>
@@ -8077,6 +7979,10 @@
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>